<commit_message>
Save User 버튼을 individual로 수정
</commit_message>
<xml_diff>
--- a/data/group_user_data.xlsx
+++ b/data/group_user_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,14 @@
           <t>testing 3</t>
         </is>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -493,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -858,10 +866,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -873,24 +879,117 @@
           <t>male</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>53</v>
+      </c>
+      <c r="E13" t="n">
+        <v>170</v>
+      </c>
+      <c r="F13" t="n">
+        <v>72</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>testuser01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Park</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>53</v>
+      </c>
+      <c r="E14" t="n">
+        <v>170</v>
+      </c>
+      <c r="F14" t="n">
+        <v>72</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>testuser02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Lee</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>48</v>
+      </c>
+      <c r="E15" t="n">
+        <v>148</v>
+      </c>
+      <c r="F15" t="n">
+        <v>56</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>testuser03</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>163.8</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>53</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>170</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>72</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>test1</t>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>TEST</t>
         </is>
       </c>
     </row>

</xml_diff>